<commit_message>
updated with our estimates
</commit_message>
<xml_diff>
--- a/PreyIngestPredict.xlsx
+++ b/PreyIngestPredict.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Intercept (A)</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Nagy 2001</t>
+  </si>
+  <si>
+    <t>Savoca et al., this study</t>
   </si>
 </sst>
 </file>
@@ -415,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D7"/>
+  <dimension ref="B1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -505,6 +508,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="2:4">
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>0.75</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Adding BMR to ADMR to R estimates
</commit_message>
<xml_diff>
--- a/PreyIngestPredict.xlsx
+++ b/PreyIngestPredict.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsavoca/Documents/Research Data/Whale research/ShirelCh2/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806F0201-A411-754E-8228-4F21EF4FAA54}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16140"/>
+    <workbookView xWindow="-920" yWindow="-21880" windowWidth="28040" windowHeight="16140" activeTab="1" xr2:uid="{7458E51B-6549-6D48-AF2B-39BBF0AD2093}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Direct estimate of R" sheetId="1" r:id="rId1"/>
+    <sheet name="BMR to R" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Intercept (A)</t>
   </si>
@@ -42,9 +46,6 @@
     <t>Innes et al. 1987</t>
   </si>
   <si>
-    <t>Tamura and Ohsumi 2000, method 1</t>
-  </si>
-  <si>
     <t>Reilly et al. 2004</t>
   </si>
   <si>
@@ -57,19 +58,46 @@
     <t>Nagy 2001</t>
   </si>
   <si>
-    <t>Savoca et al., this study (lower bound)</t>
-  </si>
-  <si>
-    <t>Savoca et al., this study (upper bound)</t>
-  </si>
-  <si>
-    <t>Savoca et al., this study (best estimate)</t>
+    <t>Mass (M) in kg</t>
+  </si>
+  <si>
+    <t>Klumov 1963; Tamura and Ohsumi 2000, method 1</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Balaenoptera bonaerensis</t>
+  </si>
+  <si>
+    <t>Balaenoptera edeni</t>
+  </si>
+  <si>
+    <t>Balaenoptera borealis</t>
+  </si>
+  <si>
+    <t>Megaptera novaeangliae</t>
+  </si>
+  <si>
+    <t>Balaenoptera physalus</t>
+  </si>
+  <si>
+    <t>Balaenoptera musculus</t>
+  </si>
+  <si>
+    <t>M_kg</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Balaenoptera acutorostrata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -107,9 +135,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -170,7 +199,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -222,7 +251,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -416,28 +445,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482BAB4E-D268-1941-9A45-39293D1E956C}">
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,114 +475,284 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.1</v>
       </c>
       <c r="B2">
         <v>0.8</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2">
+        <v>5000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.42</v>
       </c>
       <c r="B3">
         <v>0.67</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="C3">
+        <v>5000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="C4">
+        <v>5000</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1.66</v>
       </c>
       <c r="B5">
         <v>0.55900000000000005</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="C5">
+        <v>5000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.123</v>
       </c>
       <c r="B6">
         <v>0.8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6">
+        <v>5000</v>
+      </c>
+      <c r="D6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.17</v>
       </c>
       <c r="B7">
         <v>0.77300000000000002</v>
       </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>24.596219999999999</v>
-      </c>
-      <c r="B8">
-        <v>0.75</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>5.2556029999999998</v>
-      </c>
-      <c r="B9">
-        <v>0.75</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>8.4089639999999992</v>
-      </c>
-      <c r="B10">
-        <v>0.75</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
+      <c r="C7">
+        <v>5000</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D76CF6D-A10B-A345-A62B-5EBA7E09DE01}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>6800</v>
+      </c>
+      <c r="C2">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>6700</v>
+      </c>
+      <c r="C3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>13000.37</v>
+      </c>
+      <c r="C4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>16916.669999999998</v>
+      </c>
+      <c r="C5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>36000</v>
+      </c>
+      <c r="C6">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>53000</v>
+      </c>
+      <c r="C7">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>93000</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding changes while in Antarctica
</commit_message>
<xml_diff>
--- a/PreyIngestPredict.xlsx
+++ b/PreyIngestPredict.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsavoca/Documents/Research Data/Whale research/ShirelCh2/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0716604-D546-5D49-8BB7-54B2EA6E76DD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Direct estimate of R" sheetId="1" r:id="rId1"/>
     <sheet name="BMR to R" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -459,21 +459,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -481,7 +481,7 @@
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,7 +495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -509,7 +509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.42</v>
       </c>
@@ -523,7 +523,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3.5000000000000003E-2</v>
       </c>
@@ -537,7 +537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1.66</v>
       </c>
@@ -551,7 +551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.123</v>
       </c>
@@ -565,7 +565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.17</v>
       </c>
@@ -579,118 +579,118 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>24.596219999999999</v>
       </c>
       <c r="B8" s="3">
         <v>0.75</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>5.2556029999999998</v>
       </c>
       <c r="B9" s="3">
         <v>0.75</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>8.4089639999999992</v>
       </c>
       <c r="B10" s="3">
         <v>0.75</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
     </row>
   </sheetData>
@@ -704,19 +704,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -727,7 +727,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -738,7 +738,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -749,7 +749,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -760,7 +760,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -771,7 +771,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -782,7 +782,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -793,7 +793,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>

</xml_diff>